<commit_message>
limpieza asento y ñ
</commit_message>
<xml_diff>
--- a/ejemplo con campos.xlsx
+++ b/ejemplo con campos.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
-  <si>
-    <t>Doc</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -33,9 +30,6 @@
     <t>CP</t>
   </si>
   <si>
-    <t>PCIA</t>
-  </si>
-  <si>
     <t>idCliente</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>VICENTE LOPEZ  538</t>
   </si>
   <si>
-    <t>BUENOS AIRES</t>
-  </si>
-  <si>
     <t>ROSARIO</t>
   </si>
   <si>
@@ -76,6 +67,12 @@
   </si>
   <si>
     <t>RAFAELA</t>
+  </si>
+  <si>
+    <t>pesoenvio</t>
+  </si>
+  <si>
+    <t>PRODUCTO</t>
   </si>
 </sst>
 </file>
@@ -130,51 +127,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -184,34 +142,32 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,241 +473,242 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="E3" s="8">
         <v>2000</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>10</v>
+      <c r="F3" s="8">
+        <v>1.5</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="8">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8">
         <v>1001</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>15</v>
+      <c r="F4" s="8">
+        <v>2</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="8">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8">
         <v>3560</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>15</v>
+      <c r="F5" s="8">
+        <v>3</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="8">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="E6" s="8">
         <v>2001</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
+      <c r="F6" s="8">
+        <v>1</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="8">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8">
         <v>3000</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>10</v>
+      <c r="F7" s="8">
+        <v>2.8</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8">
         <v>2300</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
+      <c r="F8" s="8">
+        <v>3</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="8">
         <v>17</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="8">
         <v>1000</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>10</v>
+      <c r="F9" s="8">
+        <v>1</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="8">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="8">
         <v>1001</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
+      <c r="F10" s="8">
+        <v>2</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>

</xml_diff>